<commit_message>
Different CNN architecture comparison for CIFAR10
</commit_message>
<xml_diff>
--- a/CNN Architecture Comparison.xlsx
+++ b/CNN Architecture Comparison.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="MNIST_Network" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="CIFAR - 10" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>Accuracy</t>
   </si>
@@ -56,6 +57,27 @@
   </si>
   <si>
     <t>Architecture-5</t>
+  </si>
+  <si>
+    <t>optimizer</t>
+  </si>
+  <si>
+    <t>activation</t>
+  </si>
+  <si>
+    <t>rmsprop</t>
+  </si>
+  <si>
+    <t>relu</t>
+  </si>
+  <si>
+    <t>adam</t>
+  </si>
+  <si>
+    <t>LeakyReLU</t>
+  </si>
+  <si>
+    <t>rmsprop learnign rate 0.0001</t>
   </si>
 </sst>
 </file>
@@ -88,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -104,6 +126,12 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -113,6 +141,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -512,4 +544,229 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="9" max="9" width="19.43"/>
+  </cols>
+  <sheetData>
+    <row r="2">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2">
+        <v>67.0</v>
+      </c>
+      <c r="C3" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="I3" s="4">
+        <v>305162.0</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2">
+        <v>95.18</v>
+      </c>
+      <c r="C4" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="F4" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="I4" s="6">
+        <v>314410.0</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2">
+        <v>92.77</v>
+      </c>
+      <c r="C5" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>314410.0</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2">
+        <v>90.24</v>
+      </c>
+      <c r="C6" s="3">
+        <v>50.0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="I6" s="6">
+        <v>162442.0</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="2">
+        <v>92.29</v>
+      </c>
+      <c r="C7" s="2">
+        <v>50.0</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E7" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="I7" s="6">
+        <v>314410.0</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>